<commit_message>
Update Mahasiswa and KRS Import
</commit_message>
<xml_diff>
--- a/public/template/template_import_mahasiswa.xlsx
+++ b/public/template/template_import_mahasiswa.xlsx
@@ -1132,7 +1132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="209">
   <si>
     <t>NIM</t>
   </si>
@@ -1380,6 +1380,9 @@
     <t>Institut Teknologi Bandung</t>
   </si>
   <si>
+    <t>MO-002</t>
+  </si>
+  <si>
     <t>MANAJEMEN REKAYASA KONSTRUKSI</t>
   </si>
   <si>
@@ -1452,9 +1455,6 @@
     <t>Universitas Pendidikan Indonesia</t>
   </si>
   <si>
-    <t>MO-002</t>
-  </si>
-  <si>
     <t>ALI FAHMI</t>
   </si>
   <si>
@@ -1482,160 +1482,283 @@
     <t>Universitas Negeri Semarang</t>
   </si>
   <si>
+    <t>RINA SETIAWATI</t>
+  </si>
+  <si>
+    <t>YOGYAKARTA</t>
+  </si>
+  <si>
+    <t>1997-04-10</t>
+  </si>
+  <si>
+    <t>175753231323547</t>
+  </si>
+  <si>
+    <t>123456123456126</t>
+  </si>
+  <si>
+    <t>rinap@gmail.com</t>
+  </si>
+  <si>
+    <t>BAHRI AYAH</t>
+  </si>
+  <si>
+    <t>RINA IBU</t>
+  </si>
+  <si>
+    <t>MARYAM</t>
+  </si>
+  <si>
+    <t>Universitas Islam Indonesia</t>
+  </si>
+  <si>
+    <t>ANDI WIDYAWAN</t>
+  </si>
+  <si>
+    <t>SURABAYA</t>
+  </si>
+  <si>
+    <t>1995-05-12</t>
+  </si>
+  <si>
+    <t>128965434123450</t>
+  </si>
+  <si>
+    <t>123456123456127</t>
+  </si>
+  <si>
+    <t>andiw@gmail.com</t>
+  </si>
+  <si>
+    <t>1234567890123460</t>
+  </si>
+  <si>
+    <t>ALI AYAH</t>
+  </si>
+  <si>
+    <t>YASMIN IBU</t>
+  </si>
+  <si>
+    <t>FAHMI</t>
+  </si>
+  <si>
+    <t>Universitas Negeri Surabaya</t>
+  </si>
+  <si>
+    <t>DINA SARI</t>
+  </si>
+  <si>
+    <t>MEDAN</t>
+  </si>
+  <si>
+    <t>1998-02-18</t>
+  </si>
+  <si>
+    <t>123245678923450</t>
+  </si>
+  <si>
+    <t>123456123456128</t>
+  </si>
+  <si>
+    <t>dina@gmail.com</t>
+  </si>
+  <si>
+    <t>SAMSUL AYAH</t>
+  </si>
+  <si>
+    <t>AINI IBU</t>
+  </si>
+  <si>
+    <t>SYAHRUL</t>
+  </si>
+  <si>
+    <t>Universitas Sumatera Utara</t>
+  </si>
+  <si>
+    <t>HENDRA ANWAR</t>
+  </si>
+  <si>
+    <t>PALEMBANG</t>
+  </si>
+  <si>
+    <t>1999-06-24</t>
+  </si>
+  <si>
+    <t>123456723443277</t>
+  </si>
+  <si>
+    <t>123456123456129</t>
+  </si>
+  <si>
+    <t>hendra@gmail.com</t>
+  </si>
+  <si>
+    <t>JANI AYAH</t>
+  </si>
+  <si>
+    <t>HANI IBU</t>
+  </si>
+  <si>
+    <t>JUNAIDI</t>
+  </si>
+  <si>
+    <t>Universitas Sriwijaya</t>
+  </si>
+  <si>
+    <t>SANDRA PUTRI</t>
+  </si>
+  <si>
+    <t>1996-07-19</t>
+  </si>
+  <si>
+    <t>174554789045544</t>
+  </si>
+  <si>
+    <t>123456123456130</t>
+  </si>
+  <si>
+    <t>sandraputri@gmail.com</t>
+  </si>
+  <si>
+    <t>AMAN AYAH</t>
+  </si>
+  <si>
+    <t>SITI IBU</t>
+  </si>
+  <si>
+    <t>RAHMAT</t>
+  </si>
+  <si>
+    <t>Universitas Pendidikan Bandung</t>
+  </si>
+  <si>
+    <t>9999999910</t>
+  </si>
+  <si>
+    <t>YAYAT 234</t>
+  </si>
+  <si>
+    <t>123456789132123</t>
+  </si>
+  <si>
+    <t>02137654321</t>
+  </si>
+  <si>
+    <t>dimasd132y99@gmail.com</t>
+  </si>
+  <si>
+    <t>BUDI 24</t>
+  </si>
+  <si>
+    <t>1234567823234214223</t>
+  </si>
+  <si>
+    <t>sa132iayudha262@gmail.com</t>
+  </si>
+  <si>
     <t>TE-003</t>
   </si>
   <si>
-    <t>RINA SETIAWATI</t>
-  </si>
-  <si>
-    <t>YOGYAKARTA</t>
-  </si>
-  <si>
-    <t>1997-04-10</t>
-  </si>
-  <si>
-    <t>175753231323547</t>
-  </si>
-  <si>
-    <t>123456123456126</t>
-  </si>
-  <si>
-    <t>rinap@gmail.com</t>
-  </si>
-  <si>
-    <t>BAHRI AYAH</t>
-  </si>
-  <si>
-    <t>RINA IBU</t>
-  </si>
-  <si>
-    <t>MARYAM</t>
-  </si>
-  <si>
-    <t>Universitas Islam Indonesia</t>
-  </si>
-  <si>
-    <t>ANDI WIDYAWAN</t>
-  </si>
-  <si>
-    <t>SURABAYA</t>
-  </si>
-  <si>
-    <t>1995-05-12</t>
-  </si>
-  <si>
-    <t>128965434123450</t>
-  </si>
-  <si>
-    <t>123456123456127</t>
-  </si>
-  <si>
-    <t>andiw@gmail.com</t>
-  </si>
-  <si>
-    <t>1234567890123460</t>
-  </si>
-  <si>
-    <t>ALI AYAH</t>
-  </si>
-  <si>
-    <t>YASMIN IBU</t>
-  </si>
-  <si>
-    <t>FAHMI</t>
-  </si>
-  <si>
-    <t>Universitas Negeri Surabaya</t>
-  </si>
-  <si>
-    <t>DINA SARI</t>
-  </si>
-  <si>
-    <t>MEDAN</t>
-  </si>
-  <si>
-    <t>1998-02-18</t>
-  </si>
-  <si>
-    <t>123245678923450</t>
-  </si>
-  <si>
-    <t>123456123456128</t>
-  </si>
-  <si>
-    <t>dina@gmail.com</t>
-  </si>
-  <si>
-    <t>SAMSUL AYAH</t>
-  </si>
-  <si>
-    <t>AINI IBU</t>
-  </si>
-  <si>
-    <t>SYAHRUL</t>
-  </si>
-  <si>
-    <t>Universitas Sumatera Utara</t>
-  </si>
-  <si>
-    <t>HENDRA ANWAR</t>
-  </si>
-  <si>
-    <t>PALEMBANG</t>
-  </si>
-  <si>
-    <t>1999-06-24</t>
-  </si>
-  <si>
-    <t>123456723443277</t>
-  </si>
-  <si>
-    <t>123456123456129</t>
-  </si>
-  <si>
-    <t>hendra@gmail.com</t>
-  </si>
-  <si>
-    <t>JANI AYAH</t>
-  </si>
-  <si>
-    <t>HANI IBU</t>
-  </si>
-  <si>
-    <t>JUNAIDI</t>
-  </si>
-  <si>
     <t>MSDM-004</t>
   </si>
   <si>
-    <t>Universitas Sriwijaya</t>
-  </si>
-  <si>
-    <t>SANDRA PUTRI</t>
-  </si>
-  <si>
-    <t>1996-07-19</t>
-  </si>
-  <si>
-    <t>174554789045544</t>
-  </si>
-  <si>
-    <t>123456123456130</t>
-  </si>
-  <si>
-    <t>sandraputri@gmail.com</t>
-  </si>
-  <si>
-    <t>AMAN AYAH</t>
-  </si>
-  <si>
-    <t>SITI IBU</t>
-  </si>
-  <si>
-    <t>RAHMAT</t>
-  </si>
-  <si>
-    <t>Universitas Pendidikan Bandung</t>
+    <t>SITI 234</t>
+  </si>
+  <si>
+    <t>213231312445551</t>
+  </si>
+  <si>
+    <t>ba123ar@gmail.com</t>
+  </si>
+  <si>
+    <t>ALI 432</t>
+  </si>
+  <si>
+    <t>12335645601132</t>
+  </si>
+  <si>
+    <t>an123tian20@gmail.com</t>
+  </si>
+  <si>
+    <t>RINA 423</t>
+  </si>
+  <si>
+    <t>17575476523547</t>
+  </si>
+  <si>
+    <t>987655644324</t>
+  </si>
+  <si>
+    <t>rinap132@gmail.com</t>
+  </si>
+  <si>
+    <t>ANDI 456</t>
+  </si>
+  <si>
+    <t>1289655045629</t>
+  </si>
+  <si>
+    <t>andiw312@gmail.com</t>
+  </si>
+  <si>
+    <t>DINA 574</t>
+  </si>
+  <si>
+    <t>123245632476450</t>
+  </si>
+  <si>
+    <t>dina132@gmail.com</t>
+  </si>
+  <si>
+    <t>HENDRA 324</t>
+  </si>
+  <si>
+    <t>123456765742277</t>
+  </si>
+  <si>
+    <t>987213654327</t>
+  </si>
+  <si>
+    <t>hendr132a@gmail.com</t>
+  </si>
+  <si>
+    <t>SANDRA 76</t>
+  </si>
+  <si>
+    <t>1745590878544</t>
+  </si>
+  <si>
+    <t>sandra123putri@gmail.com</t>
+  </si>
+  <si>
+    <t>SANDRA 2133</t>
+  </si>
+  <si>
+    <t>17454320878544</t>
+  </si>
+  <si>
+    <t>9876435224328</t>
+  </si>
+  <si>
+    <t>123456133323456130</t>
+  </si>
+  <si>
+    <t>sandra132putri@gmail.com</t>
+  </si>
+  <si>
+    <t>SANDRA 123</t>
+  </si>
+  <si>
+    <t>174559087668544</t>
+  </si>
+  <si>
+    <t>98762134354328</t>
+  </si>
+  <si>
+    <t>12343356123456130</t>
+  </si>
+  <si>
+    <t>sandrapu132tri@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1648,7 +1771,7 @@
     <numFmt numFmtId="178" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1665,6 +1788,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
@@ -1705,6 +1834,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+    </font>
+    <font>
       <sz val="10.5"/>
       <name val="Consolas"/>
       <charset val="134"/>
@@ -1712,6 +1848,12 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
       <charset val="134"/>
     </font>
     <font>
@@ -2227,137 +2369,137 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2373,61 +2515,85 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="58" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2963,10 +3129,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AW11"/>
+  <dimension ref="A1:AW21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AF10" sqref="AF10"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2978,7 +3144,7 @@
     <col min="5" max="5" width="16.7142857142857" customWidth="1"/>
     <col min="6" max="6" width="25.4285714285714" customWidth="1"/>
     <col min="7" max="7" width="11.4285714285714"/>
-    <col min="8" max="8" width="10.5714285714286"/>
+    <col min="8" max="8" width="12.8571428571429"/>
     <col min="9" max="9" width="18" customWidth="1"/>
     <col min="10" max="10" width="12.8571428571429"/>
     <col min="11" max="11" width="17.2857142857143" customWidth="1"/>
@@ -3027,124 +3193,124 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="9" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="10" t="s">
+      <c r="P1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="Q1" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="10" t="s">
+      <c r="R1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="10" t="s">
+      <c r="S1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="10" t="s">
+      <c r="T1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="10" t="s">
+      <c r="U1" s="11" t="s">
         <v>20</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="10" t="s">
+      <c r="W1" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="10" t="s">
+      <c r="X1" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="10" t="s">
+      <c r="Y1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="Z1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="10" t="s">
+      <c r="AA1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="10" t="s">
+      <c r="AB1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="10" t="s">
+      <c r="AC1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="10" t="s">
+      <c r="AD1" s="11" t="s">
         <v>29</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="10" t="s">
+      <c r="AF1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="10" t="s">
+      <c r="AG1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="10" t="s">
+      <c r="AH1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="10" t="s">
+      <c r="AI1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="10" t="s">
+      <c r="AJ1" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="10" t="s">
+      <c r="AK1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="10" t="s">
+      <c r="AL1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="10" t="s">
+      <c r="AM1" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="10" t="s">
+      <c r="AN1" s="11" t="s">
         <v>39</v>
       </c>
       <c r="AO1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="16" t="s">
+      <c r="AP1" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" s="17" t="s">
+      <c r="AQ1" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" s="17" t="s">
+      <c r="AR1" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="17" t="s">
+      <c r="AS1" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" s="17" t="s">
+      <c r="AT1" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" s="17" t="s">
+      <c r="AU1" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" s="6" t="s">
+      <c r="AV1" s="7" t="s">
         <v>47</v>
       </c>
       <c r="AW1" s="1" t="s">
@@ -3176,7 +3342,7 @@
       <c r="H2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="I2" s="12" t="s">
         <v>56</v>
       </c>
       <c r="J2" s="2" t="s">
@@ -3209,10 +3375,10 @@
       <c r="S2" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="T2" s="22" t="s">
+      <c r="T2" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="U2" s="12" t="s">
+      <c r="U2" s="15" t="s">
         <v>65</v>
       </c>
       <c r="V2" s="2" t="s">
@@ -3255,43 +3421,43 @@
       <c r="AI2" s="2">
         <v>13</v>
       </c>
-      <c r="AJ2" s="15" t="s">
+      <c r="AJ2" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="AK2" s="15" t="s">
+      <c r="AK2" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="AL2" s="15" t="s">
+      <c r="AL2" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="AM2" s="15" t="s">
+      <c r="AM2" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="AN2" s="15" t="s">
+      <c r="AN2" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="AO2" s="18" t="s">
+      <c r="AO2" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="AP2" s="19" t="s">
+      <c r="AP2" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="AQ2" s="20" t="s">
+      <c r="AQ2" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="AR2" s="20" t="s">
+      <c r="AR2" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="AS2" s="20" t="s">
+      <c r="AS2" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="AT2" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="AU2" s="15" t="s">
+      <c r="AT2" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="AV2" s="15">
+      <c r="AU2" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="AV2" s="20">
         <v>1</v>
       </c>
       <c r="AW2" s="2">
@@ -3303,19 +3469,19 @@
         <v>9999999991</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="23" t="s">
-        <v>86</v>
+      <c r="F3" s="30" t="s">
+        <v>87</v>
       </c>
       <c r="G3" s="3">
         <v>1</v>
@@ -3326,8 +3492,8 @@
       <c r="I3" s="3">
         <v>4</v>
       </c>
-      <c r="J3" s="23" t="s">
-        <v>87</v>
+      <c r="J3" s="30" t="s">
+        <v>88</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>58</v>
@@ -3335,7 +3501,7 @@
       <c r="L3" s="3">
         <v>1</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M3" s="13">
         <v>43728</v>
       </c>
       <c r="N3" s="3">
@@ -3359,18 +3525,18 @@
       <c r="T3" s="3">
         <v>81234567890</v>
       </c>
-      <c r="U3" s="13" t="s">
-        <v>88</v>
+      <c r="U3" s="16" t="s">
+        <v>89</v>
       </c>
       <c r="V3" s="3">
         <v>1</v>
       </c>
       <c r="W3" s="3"/>
-      <c r="X3" s="23" t="s">
-        <v>89</v>
+      <c r="X3" s="30" t="s">
+        <v>90</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="Z3" s="2" t="s">
         <v>69</v>
@@ -3384,11 +3550,11 @@
       <c r="AC3" s="3">
         <v>11</v>
       </c>
-      <c r="AD3" s="23" t="s">
-        <v>89</v>
+      <c r="AD3" s="30" t="s">
+        <v>90</v>
       </c>
       <c r="AE3" s="3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="AF3" s="2" t="s">
         <v>72</v>
@@ -3403,9 +3569,9 @@
         <v>11</v>
       </c>
       <c r="AJ3" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="AK3" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="AK3" s="20" t="s">
         <v>74</v>
       </c>
       <c r="AL3" s="3">
@@ -3414,29 +3580,29 @@
       <c r="AM3" s="3">
         <v>4</v>
       </c>
-      <c r="AN3" s="15" t="s">
+      <c r="AN3" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="AO3" s="18" t="s">
+      <c r="AO3" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="AP3" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="AQ3" s="21">
+      <c r="AP3" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ3" s="28">
         <v>21</v>
       </c>
-      <c r="AR3" s="21">
+      <c r="AR3" s="28">
         <v>2001</v>
       </c>
-      <c r="AS3" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="AT3" s="18" t="s">
-        <v>77</v>
+      <c r="AS3" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="AT3" s="27" t="s">
+        <v>82</v>
       </c>
       <c r="AU3" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AV3" s="3">
         <v>1</v>
@@ -3450,19 +3616,19 @@
         <v>9999999992</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>51</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F4" s="23" t="s">
         <v>99</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>100</v>
       </c>
       <c r="G4" s="3">
         <v>1</v>
@@ -3473,8 +3639,8 @@
       <c r="I4" s="3">
         <v>11</v>
       </c>
-      <c r="J4" s="23" t="s">
-        <v>100</v>
+      <c r="J4" s="30" t="s">
+        <v>101</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>58</v>
@@ -3482,7 +3648,7 @@
       <c r="L4" s="3">
         <v>1</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M4" s="13">
         <v>43840</v>
       </c>
       <c r="N4" s="3">
@@ -3506,18 +3672,18 @@
       <c r="T4" s="3">
         <v>82345678901</v>
       </c>
-      <c r="U4" s="14" t="s">
-        <v>101</v>
+      <c r="U4" s="17" t="s">
+        <v>102</v>
       </c>
       <c r="V4" s="3">
         <v>0</v>
       </c>
       <c r="W4" s="3"/>
-      <c r="X4" s="23" t="s">
-        <v>89</v>
+      <c r="X4" s="30" t="s">
+        <v>90</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="Z4" s="2" t="s">
         <v>69</v>
@@ -3531,11 +3697,11 @@
       <c r="AC4" s="3">
         <v>12</v>
       </c>
-      <c r="AD4" s="23" t="s">
-        <v>89</v>
+      <c r="AD4" s="30" t="s">
+        <v>90</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AF4" s="2" t="s">
         <v>72</v>
@@ -3550,9 +3716,9 @@
         <v>12</v>
       </c>
       <c r="AJ4" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="AK4" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK4" s="20" t="s">
         <v>74</v>
       </c>
       <c r="AL4" s="3">
@@ -3561,29 +3727,29 @@
       <c r="AM4" s="3">
         <v>11</v>
       </c>
-      <c r="AN4" s="15" t="s">
+      <c r="AN4" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="AO4" s="18" t="s">
+      <c r="AO4" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="AP4" s="21" t="s">
+      <c r="AP4" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="AQ4" s="21">
+      <c r="AQ4" s="28">
         <v>21</v>
       </c>
-      <c r="AR4" s="21">
+      <c r="AR4" s="28">
         <v>2002</v>
       </c>
-      <c r="AS4" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="AT4" s="18" t="s">
+      <c r="AS4" s="28" t="s">
         <v>106</v>
       </c>
+      <c r="AT4" s="27" t="s">
+        <v>82</v>
+      </c>
       <c r="AU4" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AV4" s="3">
         <v>2</v>
@@ -3608,7 +3774,7 @@
       <c r="E5" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="30" t="s">
         <v>110</v>
       </c>
       <c r="G5" s="3">
@@ -3620,7 +3786,7 @@
       <c r="I5" s="3">
         <v>13</v>
       </c>
-      <c r="J5" s="23" t="s">
+      <c r="J5" s="30" t="s">
         <v>111</v>
       </c>
       <c r="K5" s="3" t="s">
@@ -3629,11 +3795,11 @@
       <c r="L5" s="3">
         <v>1</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M5" s="13">
         <v>43707</v>
       </c>
       <c r="N5" s="3">
-        <v>20222</v>
+        <v>20221</v>
       </c>
       <c r="O5" s="3" t="s">
         <v>61</v>
@@ -3653,15 +3819,15 @@
       <c r="T5" s="3">
         <v>83456789012</v>
       </c>
-      <c r="U5" s="14" t="s">
+      <c r="U5" s="17" t="s">
         <v>112</v>
       </c>
       <c r="V5" s="3">
         <v>1</v>
       </c>
       <c r="W5" s="3"/>
-      <c r="X5" s="23" t="s">
-        <v>89</v>
+      <c r="X5" s="30" t="s">
+        <v>90</v>
       </c>
       <c r="Y5" s="3" t="s">
         <v>113</v>
@@ -3678,8 +3844,8 @@
       <c r="AC5" s="3">
         <v>14</v>
       </c>
-      <c r="AD5" s="23" t="s">
-        <v>89</v>
+      <c r="AD5" s="30" t="s">
+        <v>90</v>
       </c>
       <c r="AE5" s="3" t="s">
         <v>114</v>
@@ -3697,9 +3863,9 @@
         <v>12</v>
       </c>
       <c r="AJ5" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="AK5" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK5" s="20" t="s">
         <v>74</v>
       </c>
       <c r="AL5" s="3">
@@ -3708,29 +3874,29 @@
       <c r="AM5" s="3">
         <v>6</v>
       </c>
-      <c r="AN5" s="15" t="s">
+      <c r="AN5" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="AO5" s="18" t="s">
+      <c r="AO5" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="AP5" s="21" t="s">
+      <c r="AP5" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="AQ5" s="21">
+      <c r="AQ5" s="28">
         <v>21</v>
       </c>
-      <c r="AR5" s="21">
+      <c r="AR5" s="28">
         <v>2003</v>
       </c>
-      <c r="AS5" s="21" t="s">
+      <c r="AS5" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="AT5" s="18" t="s">
-        <v>116</v>
+      <c r="AT5" s="27" t="s">
+        <v>82</v>
       </c>
       <c r="AU5" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AV5" s="3">
         <v>3</v>
@@ -3744,19 +3910,19 @@
         <v>9999999994</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" s="30" t="s">
         <v>119</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F6" s="23" t="s">
-        <v>120</v>
       </c>
       <c r="G6" s="3">
         <v>2</v>
@@ -3767,8 +3933,8 @@
       <c r="I6" s="3">
         <v>15</v>
       </c>
-      <c r="J6" s="23" t="s">
-        <v>121</v>
+      <c r="J6" s="30" t="s">
+        <v>120</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>58</v>
@@ -3776,7 +3942,7 @@
       <c r="L6" s="3">
         <v>1</v>
       </c>
-      <c r="M6" s="5">
+      <c r="M6" s="13">
         <v>43348</v>
       </c>
       <c r="N6" s="3">
@@ -3800,18 +3966,18 @@
       <c r="T6" s="3">
         <v>84567890123</v>
       </c>
-      <c r="U6" s="13" t="s">
-        <v>122</v>
+      <c r="U6" s="16" t="s">
+        <v>121</v>
       </c>
       <c r="V6" s="3">
         <v>0</v>
       </c>
       <c r="W6" s="3"/>
-      <c r="X6" s="23" t="s">
-        <v>89</v>
+      <c r="X6" s="30" t="s">
+        <v>90</v>
       </c>
       <c r="Y6" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Z6" s="2" t="s">
         <v>69</v>
@@ -3825,11 +3991,11 @@
       <c r="AC6" s="3">
         <v>12</v>
       </c>
-      <c r="AD6" s="23" t="s">
-        <v>89</v>
+      <c r="AD6" s="30" t="s">
+        <v>90</v>
       </c>
       <c r="AE6" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="AF6" s="2" t="s">
         <v>72</v>
@@ -3844,9 +4010,9 @@
         <v>11</v>
       </c>
       <c r="AJ6" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="AK6" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="AK6" s="20" t="s">
         <v>74</v>
       </c>
       <c r="AL6" s="3">
@@ -3855,29 +4021,29 @@
       <c r="AM6" s="3">
         <v>12</v>
       </c>
-      <c r="AN6" s="15" t="s">
+      <c r="AN6" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="AO6" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="AP6" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="AQ6" s="21">
+      <c r="AO6" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="AP6" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ6" s="28">
         <v>21</v>
       </c>
-      <c r="AR6" s="21">
+      <c r="AR6" s="28">
         <v>2004</v>
       </c>
-      <c r="AS6" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="AT6" s="18" t="s">
-        <v>106</v>
+      <c r="AS6" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="AT6" s="27" t="s">
+        <v>82</v>
       </c>
       <c r="AU6" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AV6" s="3">
         <v>2</v>
@@ -3891,19 +4057,19 @@
         <v>9999999995</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="4" t="s">
         <v>128</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>129</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="23" t="s">
-        <v>130</v>
+      <c r="F7" s="30" t="s">
+        <v>129</v>
       </c>
       <c r="G7" s="3">
         <v>1</v>
@@ -3914,8 +4080,8 @@
       <c r="I7" s="3">
         <v>9</v>
       </c>
-      <c r="J7" s="23" t="s">
-        <v>131</v>
+      <c r="J7" s="30" t="s">
+        <v>130</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>58</v>
@@ -3923,11 +4089,11 @@
       <c r="L7" s="3">
         <v>1</v>
       </c>
-      <c r="M7" s="5">
+      <c r="M7" s="13">
         <v>43850</v>
       </c>
       <c r="N7" s="3">
-        <v>20222</v>
+        <v>20221</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>61</v>
@@ -3947,18 +4113,18 @@
       <c r="T7" s="3">
         <v>85678901234</v>
       </c>
-      <c r="U7" s="13" t="s">
+      <c r="U7" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="V7" s="3">
+        <v>1</v>
+      </c>
+      <c r="W7" s="3"/>
+      <c r="X7" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="V7" s="3">
-        <v>1</v>
-      </c>
-      <c r="W7" s="3"/>
-      <c r="X7" s="23" t="s">
+      <c r="Y7" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="Y7" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="Z7" s="2" t="s">
         <v>69</v>
@@ -3972,11 +4138,11 @@
       <c r="AC7" s="3">
         <v>12</v>
       </c>
-      <c r="AD7" s="23" t="s">
-        <v>133</v>
+      <c r="AD7" s="30" t="s">
+        <v>132</v>
       </c>
       <c r="AE7" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AF7" s="2" t="s">
         <v>72</v>
@@ -3991,9 +4157,9 @@
         <v>14</v>
       </c>
       <c r="AJ7" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="AK7" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="AK7" s="20" t="s">
         <v>74</v>
       </c>
       <c r="AL7" s="3">
@@ -4005,26 +4171,26 @@
       <c r="AN7" s="3">
         <v>12</v>
       </c>
-      <c r="AO7" s="18" t="s">
+      <c r="AO7" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP7" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ7" s="28">
+        <v>21</v>
+      </c>
+      <c r="AR7" s="28">
+        <v>2005</v>
+      </c>
+      <c r="AS7" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="AT7" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="AP7" s="21" t="s">
-        <v>78</v>
-      </c>
-      <c r="AQ7" s="21">
-        <v>21</v>
-      </c>
-      <c r="AR7" s="21">
-        <v>2005</v>
-      </c>
-      <c r="AS7" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="AT7" s="18" t="s">
-        <v>77</v>
-      </c>
       <c r="AU7" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AV7" s="3">
         <v>1</v>
@@ -4038,19 +4204,19 @@
         <v>9999999996</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F8" s="30" t="s">
         <v>140</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F8" s="23" t="s">
-        <v>141</v>
       </c>
       <c r="G8" s="3">
         <v>1</v>
@@ -4061,8 +4227,8 @@
       <c r="I8" s="3">
         <v>4</v>
       </c>
-      <c r="J8" s="23" t="s">
-        <v>142</v>
+      <c r="J8" s="30" t="s">
+        <v>141</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>58</v>
@@ -4070,7 +4236,7 @@
       <c r="L8" s="3">
         <v>1</v>
       </c>
-      <c r="M8" s="5">
+      <c r="M8" s="13">
         <v>43539</v>
       </c>
       <c r="N8" s="3">
@@ -4094,18 +4260,18 @@
       <c r="T8" s="3">
         <v>86789012345</v>
       </c>
-      <c r="U8" s="13" t="s">
+      <c r="U8" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="V8" s="3">
+        <v>1</v>
+      </c>
+      <c r="W8" s="3"/>
+      <c r="X8" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y8" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="V8" s="3">
-        <v>1</v>
-      </c>
-      <c r="W8" s="3"/>
-      <c r="X8" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="Y8" s="3" t="s">
-        <v>144</v>
       </c>
       <c r="Z8" s="2" t="s">
         <v>69</v>
@@ -4119,11 +4285,11 @@
       <c r="AC8" s="3">
         <v>12</v>
       </c>
-      <c r="AD8" s="23" t="s">
-        <v>133</v>
+      <c r="AD8" s="30" t="s">
+        <v>132</v>
       </c>
       <c r="AE8" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="AF8" s="2" t="s">
         <v>72</v>
@@ -4138,9 +4304,9 @@
         <v>11</v>
       </c>
       <c r="AJ8" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="AK8" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="AK8" s="20" t="s">
         <v>74</v>
       </c>
       <c r="AL8" s="3">
@@ -4152,26 +4318,26 @@
       <c r="AN8" s="3">
         <v>13</v>
       </c>
-      <c r="AO8" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="AP8" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="AQ8" s="21">
+      <c r="AO8" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP8" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ8" s="28">
         <v>21</v>
       </c>
-      <c r="AR8" s="21">
+      <c r="AR8" s="28">
         <v>2006</v>
       </c>
-      <c r="AS8" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="AT8" s="18" t="s">
-        <v>116</v>
+      <c r="AS8" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="AT8" s="24" t="s">
+        <v>77</v>
       </c>
       <c r="AU8" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AV8" s="3">
         <v>1</v>
@@ -4185,19 +4351,19 @@
         <v>9999999997</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="4" t="s">
         <v>149</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>150</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="F9" s="23" t="s">
-        <v>151</v>
+      <c r="F9" s="30" t="s">
+        <v>150</v>
       </c>
       <c r="G9" s="3">
         <v>1</v>
@@ -4208,8 +4374,8 @@
       <c r="I9" s="3">
         <v>14</v>
       </c>
-      <c r="J9" s="23" t="s">
-        <v>152</v>
+      <c r="J9" s="30" t="s">
+        <v>151</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>58</v>
@@ -4217,11 +4383,11 @@
       <c r="L9" s="3">
         <v>1</v>
       </c>
-      <c r="M9" s="5">
+      <c r="M9" s="13">
         <v>43889</v>
       </c>
       <c r="N9" s="3">
-        <v>20222</v>
+        <v>20221</v>
       </c>
       <c r="O9" s="3" t="s">
         <v>61</v>
@@ -4241,18 +4407,18 @@
       <c r="T9" s="3">
         <v>87890123456</v>
       </c>
-      <c r="U9" s="13" t="s">
-        <v>153</v>
+      <c r="U9" s="16" t="s">
+        <v>152</v>
       </c>
       <c r="V9" s="3">
         <v>0</v>
       </c>
       <c r="W9" s="3"/>
-      <c r="X9" s="23" t="s">
-        <v>133</v>
+      <c r="X9" s="30" t="s">
+        <v>132</v>
       </c>
       <c r="Y9" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="Z9" s="2" t="s">
         <v>69</v>
@@ -4266,11 +4432,11 @@
       <c r="AC9" s="3">
         <v>11</v>
       </c>
-      <c r="AD9" s="23" t="s">
-        <v>133</v>
+      <c r="AD9" s="30" t="s">
+        <v>132</v>
       </c>
       <c r="AE9" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="AF9" s="2" t="s">
         <v>72</v>
@@ -4285,9 +4451,9 @@
         <v>11</v>
       </c>
       <c r="AJ9" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="AK9" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="AK9" s="20" t="s">
         <v>74</v>
       </c>
       <c r="AL9" s="3">
@@ -4299,26 +4465,26 @@
       <c r="AN9" s="3">
         <v>12</v>
       </c>
-      <c r="AO9" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="AP9" s="21" t="s">
+      <c r="AO9" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP9" s="28" t="s">
         <v>78</v>
       </c>
-      <c r="AQ9" s="21">
+      <c r="AQ9" s="28">
         <v>21</v>
       </c>
-      <c r="AR9" s="21">
+      <c r="AR9" s="28">
         <v>2007</v>
       </c>
-      <c r="AS9" s="21" t="s">
-        <v>158</v>
-      </c>
-      <c r="AT9" s="18" t="s">
-        <v>157</v>
+      <c r="AS9" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="AT9" s="24" t="s">
+        <v>77</v>
       </c>
       <c r="AU9" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AV9" s="3">
         <v>1</v>
@@ -4332,19 +4498,19 @@
         <v>9999999998</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>51</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F10" s="23" t="s">
-        <v>161</v>
+        <v>99</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>159</v>
       </c>
       <c r="G10" s="3">
         <v>2</v>
@@ -4355,8 +4521,8 @@
       <c r="I10" s="3">
         <v>12</v>
       </c>
-      <c r="J10" s="23" t="s">
-        <v>162</v>
+      <c r="J10" s="30" t="s">
+        <v>160</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>58</v>
@@ -4364,7 +4530,7 @@
       <c r="L10" s="3">
         <v>1</v>
       </c>
-      <c r="M10" s="5">
+      <c r="M10" s="13">
         <v>43606</v>
       </c>
       <c r="N10" s="3">
@@ -4388,18 +4554,18 @@
       <c r="T10" s="3">
         <v>88901234567</v>
       </c>
-      <c r="U10" s="13" t="s">
-        <v>163</v>
+      <c r="U10" s="16" t="s">
+        <v>161</v>
       </c>
       <c r="V10" s="3">
         <v>1</v>
       </c>
       <c r="W10" s="3"/>
-      <c r="X10" s="23" t="s">
-        <v>133</v>
+      <c r="X10" s="30" t="s">
+        <v>132</v>
       </c>
       <c r="Y10" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="Z10" s="2" t="s">
         <v>69</v>
@@ -4413,11 +4579,11 @@
       <c r="AC10" s="3">
         <v>13</v>
       </c>
-      <c r="AD10" s="23" t="s">
-        <v>133</v>
+      <c r="AD10" s="30" t="s">
+        <v>132</v>
       </c>
       <c r="AE10" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AF10" s="2" t="s">
         <v>72</v>
@@ -4432,9 +4598,9 @@
         <v>11</v>
       </c>
       <c r="AJ10" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="AK10" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="AK10" s="20" t="s">
         <v>74</v>
       </c>
       <c r="AL10" s="3">
@@ -4446,26 +4612,26 @@
       <c r="AN10" s="3">
         <v>12</v>
       </c>
-      <c r="AO10" s="18" t="s">
-        <v>157</v>
-      </c>
-      <c r="AP10" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="AQ10" s="21">
+      <c r="AO10" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP10" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ10" s="28">
         <v>21</v>
       </c>
-      <c r="AR10" s="21">
+      <c r="AR10" s="28">
         <v>2008</v>
       </c>
-      <c r="AS10" s="21" t="s">
-        <v>167</v>
-      </c>
-      <c r="AT10" s="18" t="s">
-        <v>157</v>
+      <c r="AS10" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="AT10" s="24" t="s">
+        <v>77</v>
       </c>
       <c r="AU10" s="3" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="AV10" s="3">
         <v>2</v>
@@ -4475,55 +4641,1621 @@
       </c>
     </row>
     <row r="11" spans="1:49">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
-      <c r="W11" s="3"/>
-      <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="5"/>
-      <c r="AA11" s="3"/>
-      <c r="AB11" s="3"/>
-      <c r="AC11" s="3"/>
-      <c r="AD11" s="3"/>
-      <c r="AE11" s="3"/>
-      <c r="AF11" s="5"/>
-      <c r="AG11" s="3"/>
-      <c r="AH11" s="3"/>
-      <c r="AI11" s="3"/>
-      <c r="AJ11" s="3"/>
-      <c r="AK11" s="5"/>
-      <c r="AL11" s="3"/>
-      <c r="AM11" s="3"/>
-      <c r="AN11" s="3"/>
-      <c r="AO11" s="18"/>
-      <c r="AP11" s="21"/>
-      <c r="AQ11" s="21"/>
-      <c r="AR11" s="21"/>
-      <c r="AS11" s="21"/>
-      <c r="AT11" s="18"/>
-      <c r="AU11" s="3"/>
-      <c r="AV11" s="3"/>
-      <c r="AW11" s="3"/>
+      <c r="A11" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="L11" s="2">
+        <v>1</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="P11" s="2">
+        <v>41115</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>1</v>
+      </c>
+      <c r="R11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="S11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="T11" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="U11" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="W11" s="2"/>
+      <c r="X11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y11" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA11" s="2">
+        <v>2</v>
+      </c>
+      <c r="AB11" s="2">
+        <v>4</v>
+      </c>
+      <c r="AC11" s="2">
+        <v>13</v>
+      </c>
+      <c r="AD11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF11" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG11" s="2">
+        <v>3</v>
+      </c>
+      <c r="AH11" s="2">
+        <v>1</v>
+      </c>
+      <c r="AI11" s="2">
+        <v>13</v>
+      </c>
+      <c r="AJ11" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="AK11" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL11" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="AM11" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN11" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO11" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP11" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ11" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR11" s="26" t="s">
+        <v>80</v>
+      </c>
+      <c r="AS11" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="AT11" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="AU11" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="AV11" s="20">
+        <v>1</v>
+      </c>
+      <c r="AW11" s="2">
+        <v>7500000</v>
+      </c>
+    </row>
+    <row r="12" ht="75" spans="1:49">
+      <c r="A12" s="3">
+        <v>9999999911</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>172</v>
+      </c>
+      <c r="G12" s="3">
+        <v>1</v>
+      </c>
+      <c r="H12" s="3">
+        <v>943654321</v>
+      </c>
+      <c r="I12" s="3">
+        <v>4</v>
+      </c>
+      <c r="J12" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L12" s="3">
+        <v>1</v>
+      </c>
+      <c r="M12" s="13">
+        <v>43728</v>
+      </c>
+      <c r="N12" s="3">
+        <v>20221</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="P12" s="3">
+        <v>41115</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>1</v>
+      </c>
+      <c r="R12" s="3">
+        <v>3</v>
+      </c>
+      <c r="S12" s="3">
+        <v>2121456</v>
+      </c>
+      <c r="T12" s="3">
+        <v>81234567890</v>
+      </c>
+      <c r="U12" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="V12" s="3">
+        <v>1</v>
+      </c>
+      <c r="W12" s="3"/>
+      <c r="X12" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y12" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>2</v>
+      </c>
+      <c r="AB12" s="3">
+        <v>2</v>
+      </c>
+      <c r="AC12" s="3">
+        <v>11</v>
+      </c>
+      <c r="AD12" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE12" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF12" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG12" s="3">
+        <v>3</v>
+      </c>
+      <c r="AH12" s="3">
+        <v>2</v>
+      </c>
+      <c r="AI12" s="3">
+        <v>11</v>
+      </c>
+      <c r="AJ12" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AK12" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL12" s="3">
+        <v>3</v>
+      </c>
+      <c r="AM12" s="3">
+        <v>4</v>
+      </c>
+      <c r="AN12" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO12" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="AP12" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ12" s="28">
+        <v>21</v>
+      </c>
+      <c r="AR12" s="28">
+        <v>2001</v>
+      </c>
+      <c r="AS12" s="28" t="s">
+        <v>95</v>
+      </c>
+      <c r="AT12" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="AU12" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV12" s="3">
+        <v>1</v>
+      </c>
+      <c r="AW12" s="3">
+        <v>6000000</v>
+      </c>
+    </row>
+    <row r="13" ht="75" spans="1:49">
+      <c r="A13" s="3">
+        <v>9999999912</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="G13" s="3">
+        <v>1</v>
+      </c>
+      <c r="H13" s="3">
+        <v>9876554322</v>
+      </c>
+      <c r="I13" s="3">
+        <v>11</v>
+      </c>
+      <c r="J13" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L13" s="3">
+        <v>1</v>
+      </c>
+      <c r="M13" s="13">
+        <v>43840</v>
+      </c>
+      <c r="N13" s="3">
+        <v>20221</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="P13" s="3">
+        <v>41115</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>1</v>
+      </c>
+      <c r="R13" s="3">
+        <v>4</v>
+      </c>
+      <c r="S13" s="3">
+        <v>2121457</v>
+      </c>
+      <c r="T13" s="3">
+        <v>82345678901</v>
+      </c>
+      <c r="U13" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="V13" s="3">
+        <v>0</v>
+      </c>
+      <c r="W13" s="3"/>
+      <c r="X13" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y13" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z13" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>3</v>
+      </c>
+      <c r="AB13" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="3">
+        <v>12</v>
+      </c>
+      <c r="AD13" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE13" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AF13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG13" s="3">
+        <v>2</v>
+      </c>
+      <c r="AH13" s="3">
+        <v>3</v>
+      </c>
+      <c r="AI13" s="3">
+        <v>12</v>
+      </c>
+      <c r="AJ13" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK13" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL13" s="3">
+        <v>2</v>
+      </c>
+      <c r="AM13" s="3">
+        <v>11</v>
+      </c>
+      <c r="AN13" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO13" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="AP13" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ13" s="28">
+        <v>21</v>
+      </c>
+      <c r="AR13" s="28">
+        <v>2002</v>
+      </c>
+      <c r="AS13" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="AT13" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="AU13" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV13" s="3">
+        <v>2</v>
+      </c>
+      <c r="AW13" s="3">
+        <v>6500000</v>
+      </c>
+    </row>
+    <row r="14" ht="75" spans="1:49">
+      <c r="A14" s="3">
+        <v>9999999913</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="30" t="s">
+        <v>180</v>
+      </c>
+      <c r="G14" s="3">
+        <v>1</v>
+      </c>
+      <c r="H14" s="3">
+        <v>98235234323</v>
+      </c>
+      <c r="I14" s="3">
+        <v>13</v>
+      </c>
+      <c r="J14" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L14" s="3">
+        <v>1</v>
+      </c>
+      <c r="M14" s="13">
+        <v>43707</v>
+      </c>
+      <c r="N14" s="3">
+        <v>20221</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="P14" s="3">
+        <v>41115</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>1</v>
+      </c>
+      <c r="R14" s="3">
+        <v>5</v>
+      </c>
+      <c r="S14" s="3">
+        <v>2121458</v>
+      </c>
+      <c r="T14" s="3">
+        <v>83456789012</v>
+      </c>
+      <c r="U14" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="V14" s="3">
+        <v>1</v>
+      </c>
+      <c r="W14" s="3"/>
+      <c r="X14" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y14" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="Z14" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>2</v>
+      </c>
+      <c r="AB14" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="3">
+        <v>14</v>
+      </c>
+      <c r="AD14" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE14" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AF14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG14" s="3">
+        <v>3</v>
+      </c>
+      <c r="AH14" s="3">
+        <v>2</v>
+      </c>
+      <c r="AI14" s="3">
+        <v>12</v>
+      </c>
+      <c r="AJ14" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK14" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL14" s="3">
+        <v>2</v>
+      </c>
+      <c r="AM14" s="3">
+        <v>6</v>
+      </c>
+      <c r="AN14" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO14" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="AP14" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ14" s="28">
+        <v>21</v>
+      </c>
+      <c r="AR14" s="28">
+        <v>2003</v>
+      </c>
+      <c r="AS14" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="AT14" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="AU14" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV14" s="3">
+        <v>3</v>
+      </c>
+      <c r="AW14" s="3">
+        <v>7000000</v>
+      </c>
+    </row>
+    <row r="15" ht="75" spans="1:49">
+      <c r="A15" s="3">
+        <v>9999999914</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="30" t="s">
+        <v>183</v>
+      </c>
+      <c r="G15" s="3">
+        <v>2</v>
+      </c>
+      <c r="H15" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="I15" s="3">
+        <v>15</v>
+      </c>
+      <c r="J15" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L15" s="3">
+        <v>1</v>
+      </c>
+      <c r="M15" s="13">
+        <v>43348</v>
+      </c>
+      <c r="N15" s="3">
+        <v>20221</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="P15" s="3">
+        <v>41115</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>1</v>
+      </c>
+      <c r="R15" s="3">
+        <v>6</v>
+      </c>
+      <c r="S15" s="3">
+        <v>2121459</v>
+      </c>
+      <c r="T15" s="3">
+        <v>84567890123</v>
+      </c>
+      <c r="U15" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="V15" s="3">
+        <v>0</v>
+      </c>
+      <c r="W15" s="3"/>
+      <c r="X15" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y15" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z15" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA15" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB15" s="3">
+        <v>2</v>
+      </c>
+      <c r="AC15" s="3">
+        <v>12</v>
+      </c>
+      <c r="AD15" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="AE15" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="AF15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG15" s="3">
+        <v>4</v>
+      </c>
+      <c r="AH15" s="3">
+        <v>1</v>
+      </c>
+      <c r="AI15" s="3">
+        <v>11</v>
+      </c>
+      <c r="AJ15" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="AK15" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL15" s="3">
+        <v>3</v>
+      </c>
+      <c r="AM15" s="3">
+        <v>12</v>
+      </c>
+      <c r="AN15" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO15" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="AP15" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ15" s="28">
+        <v>21</v>
+      </c>
+      <c r="AR15" s="28">
+        <v>2004</v>
+      </c>
+      <c r="AS15" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="AT15" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="AU15" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV15" s="3">
+        <v>2</v>
+      </c>
+      <c r="AW15" s="3">
+        <v>5500000</v>
+      </c>
+    </row>
+    <row r="16" ht="75" spans="1:49">
+      <c r="A16" s="3">
+        <v>9999999915</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="30" t="s">
+        <v>187</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1</v>
+      </c>
+      <c r="H16" s="3">
+        <v>33244324</v>
+      </c>
+      <c r="I16" s="3">
+        <v>9</v>
+      </c>
+      <c r="J16" s="30" t="s">
+        <v>130</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L16" s="3">
+        <v>1</v>
+      </c>
+      <c r="M16" s="13">
+        <v>43850</v>
+      </c>
+      <c r="N16" s="3">
+        <v>20221</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="P16" s="3">
+        <v>41115</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>1</v>
+      </c>
+      <c r="R16" s="3">
+        <v>8</v>
+      </c>
+      <c r="S16" s="3">
+        <v>2121460</v>
+      </c>
+      <c r="T16" s="3">
+        <v>85678901234</v>
+      </c>
+      <c r="U16" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="V16" s="3">
+        <v>1</v>
+      </c>
+      <c r="W16" s="3"/>
+      <c r="X16" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y16" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="Z16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA16" s="3">
+        <v>2</v>
+      </c>
+      <c r="AB16" s="3">
+        <v>3</v>
+      </c>
+      <c r="AC16" s="3">
+        <v>12</v>
+      </c>
+      <c r="AD16" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="AE16" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="AF16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG16" s="3">
+        <v>4</v>
+      </c>
+      <c r="AH16" s="3">
+        <v>2</v>
+      </c>
+      <c r="AI16" s="3">
+        <v>14</v>
+      </c>
+      <c r="AJ16" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="AK16" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL16" s="3">
+        <v>1</v>
+      </c>
+      <c r="AM16" s="3">
+        <v>7</v>
+      </c>
+      <c r="AN16" s="3">
+        <v>12</v>
+      </c>
+      <c r="AO16" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="AP16" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ16" s="28">
+        <v>21</v>
+      </c>
+      <c r="AR16" s="28">
+        <v>2005</v>
+      </c>
+      <c r="AS16" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="AT16" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="AU16" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV16" s="3">
+        <v>1</v>
+      </c>
+      <c r="AW16" s="3">
+        <v>6000000</v>
+      </c>
+    </row>
+    <row r="17" ht="75" spans="1:49">
+      <c r="A17" s="3">
+        <v>9999999916</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F17" s="30" t="s">
+        <v>190</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3">
+        <v>24313213</v>
+      </c>
+      <c r="I17" s="3">
+        <v>4</v>
+      </c>
+      <c r="J17" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L17" s="3">
+        <v>1</v>
+      </c>
+      <c r="M17" s="13">
+        <v>43539</v>
+      </c>
+      <c r="N17" s="3">
+        <v>20221</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="P17" s="3">
+        <v>41115</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>1</v>
+      </c>
+      <c r="R17" s="3">
+        <v>11</v>
+      </c>
+      <c r="S17" s="3">
+        <v>2121461</v>
+      </c>
+      <c r="T17" s="3">
+        <v>86789012345</v>
+      </c>
+      <c r="U17" s="16" t="s">
+        <v>191</v>
+      </c>
+      <c r="V17" s="3">
+        <v>1</v>
+      </c>
+      <c r="W17" s="3"/>
+      <c r="X17" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y17" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA17" s="3">
+        <v>2</v>
+      </c>
+      <c r="AB17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AC17" s="3">
+        <v>12</v>
+      </c>
+      <c r="AD17" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="AE17" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="AF17" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG17" s="3">
+        <v>4</v>
+      </c>
+      <c r="AH17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AI17" s="3">
+        <v>11</v>
+      </c>
+      <c r="AJ17" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="AK17" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL17" s="3">
+        <v>2</v>
+      </c>
+      <c r="AM17" s="3">
+        <v>6</v>
+      </c>
+      <c r="AN17" s="3">
+        <v>13</v>
+      </c>
+      <c r="AO17" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="AP17" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ17" s="28">
+        <v>21</v>
+      </c>
+      <c r="AR17" s="28">
+        <v>2006</v>
+      </c>
+      <c r="AS17" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="AT17" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="AU17" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AW17" s="3">
+        <v>8000000</v>
+      </c>
+    </row>
+    <row r="18" ht="75" spans="1:49">
+      <c r="A18" s="3">
+        <v>99999999917</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="30" t="s">
+        <v>193</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+      <c r="H18" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="I18" s="3">
+        <v>14</v>
+      </c>
+      <c r="J18" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L18" s="3">
+        <v>1</v>
+      </c>
+      <c r="M18" s="13">
+        <v>43889</v>
+      </c>
+      <c r="N18" s="3">
+        <v>20221</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="P18" s="3">
+        <v>41115</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>1</v>
+      </c>
+      <c r="R18" s="3">
+        <v>13</v>
+      </c>
+      <c r="S18" s="3">
+        <v>2121462</v>
+      </c>
+      <c r="T18" s="3">
+        <v>87890123456</v>
+      </c>
+      <c r="U18" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="V18" s="3">
+        <v>0</v>
+      </c>
+      <c r="W18" s="3"/>
+      <c r="X18" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y18" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="Z18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA18" s="3">
+        <v>3</v>
+      </c>
+      <c r="AB18" s="3">
+        <v>2</v>
+      </c>
+      <c r="AC18" s="3">
+        <v>11</v>
+      </c>
+      <c r="AD18" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="AE18" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="AF18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG18" s="3">
+        <v>2</v>
+      </c>
+      <c r="AH18" s="3">
+        <v>1</v>
+      </c>
+      <c r="AI18" s="3">
+        <v>11</v>
+      </c>
+      <c r="AJ18" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="AK18" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL18" s="3">
+        <v>2</v>
+      </c>
+      <c r="AM18" s="3">
+        <v>6</v>
+      </c>
+      <c r="AN18" s="3">
+        <v>12</v>
+      </c>
+      <c r="AO18" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="AP18" s="28" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ18" s="28">
+        <v>21</v>
+      </c>
+      <c r="AR18" s="28">
+        <v>2007</v>
+      </c>
+      <c r="AS18" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="AT18" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="AU18" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV18" s="3">
+        <v>1</v>
+      </c>
+      <c r="AW18" s="3">
+        <v>6500000</v>
+      </c>
+    </row>
+    <row r="19" ht="75" spans="1:49">
+      <c r="A19" s="3">
+        <v>9999999918</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F19" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="G19" s="3">
+        <v>2</v>
+      </c>
+      <c r="H19" s="3">
+        <v>98764354328</v>
+      </c>
+      <c r="I19" s="3">
+        <v>12</v>
+      </c>
+      <c r="J19" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L19" s="3">
+        <v>1</v>
+      </c>
+      <c r="M19" s="13">
+        <v>43606</v>
+      </c>
+      <c r="N19" s="3">
+        <v>20221</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="P19" s="3">
+        <v>41115</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>1</v>
+      </c>
+      <c r="R19" s="3">
+        <v>99</v>
+      </c>
+      <c r="S19" s="3">
+        <v>2121463</v>
+      </c>
+      <c r="T19" s="3">
+        <v>88901234567</v>
+      </c>
+      <c r="U19" s="16" t="s">
+        <v>198</v>
+      </c>
+      <c r="V19" s="3">
+        <v>1</v>
+      </c>
+      <c r="W19" s="3"/>
+      <c r="X19" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y19" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="Z19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA19" s="3">
+        <v>2</v>
+      </c>
+      <c r="AB19" s="3">
+        <v>2</v>
+      </c>
+      <c r="AC19" s="3">
+        <v>13</v>
+      </c>
+      <c r="AD19" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="AE19" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="AF19" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG19" s="3">
+        <v>1</v>
+      </c>
+      <c r="AH19" s="3">
+        <v>2</v>
+      </c>
+      <c r="AI19" s="3">
+        <v>11</v>
+      </c>
+      <c r="AJ19" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="AK19" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL19" s="3">
+        <v>3</v>
+      </c>
+      <c r="AM19" s="3">
+        <v>17</v>
+      </c>
+      <c r="AN19" s="3">
+        <v>12</v>
+      </c>
+      <c r="AO19" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="AP19" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ19" s="28">
+        <v>21</v>
+      </c>
+      <c r="AR19" s="28">
+        <v>2008</v>
+      </c>
+      <c r="AS19" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="AT19" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="AU19" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV19" s="3">
+        <v>2</v>
+      </c>
+      <c r="AW19" s="3">
+        <v>7000000</v>
+      </c>
+    </row>
+    <row r="20" ht="75" spans="1:49">
+      <c r="A20" s="3">
+        <v>9999999919</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F20" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="G20" s="3">
+        <v>2</v>
+      </c>
+      <c r="H20" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="I20" s="3">
+        <v>12</v>
+      </c>
+      <c r="J20" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L20" s="3">
+        <v>1</v>
+      </c>
+      <c r="M20" s="13">
+        <v>43606</v>
+      </c>
+      <c r="N20" s="3">
+        <v>20221</v>
+      </c>
+      <c r="O20" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="P20" s="3">
+        <v>41115</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>1</v>
+      </c>
+      <c r="R20" s="3">
+        <v>99</v>
+      </c>
+      <c r="S20" s="3">
+        <v>2121463</v>
+      </c>
+      <c r="T20" s="3">
+        <v>88901234567</v>
+      </c>
+      <c r="U20" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="V20" s="3">
+        <v>1</v>
+      </c>
+      <c r="W20" s="3"/>
+      <c r="X20" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y20" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="Z20" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA20" s="3">
+        <v>2</v>
+      </c>
+      <c r="AB20" s="3">
+        <v>2</v>
+      </c>
+      <c r="AC20" s="3">
+        <v>13</v>
+      </c>
+      <c r="AD20" s="30" t="s">
+        <v>132</v>
+      </c>
+      <c r="AE20" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="AF20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AH20" s="3">
+        <v>2</v>
+      </c>
+      <c r="AI20" s="3">
+        <v>11</v>
+      </c>
+      <c r="AJ20" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="AK20" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL20" s="3">
+        <v>3</v>
+      </c>
+      <c r="AM20" s="3">
+        <v>17</v>
+      </c>
+      <c r="AN20" s="3">
+        <v>12</v>
+      </c>
+      <c r="AO20" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="AP20" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ20" s="28">
+        <v>21</v>
+      </c>
+      <c r="AR20" s="28">
+        <v>2008</v>
+      </c>
+      <c r="AS20" s="28" t="s">
+        <v>165</v>
+      </c>
+      <c r="AT20" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="AU20" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV20" s="3">
+        <v>2</v>
+      </c>
+      <c r="AW20" s="3">
+        <v>7000000</v>
+      </c>
+    </row>
+    <row r="21" ht="75" spans="1:49">
+      <c r="A21" s="5">
+        <v>9999999920</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="G21" s="5">
+        <v>2</v>
+      </c>
+      <c r="H21" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="I21" s="5">
+        <v>12</v>
+      </c>
+      <c r="J21" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="L21" s="5">
+        <v>1</v>
+      </c>
+      <c r="M21" s="14">
+        <v>43606</v>
+      </c>
+      <c r="N21" s="5">
+        <v>20221</v>
+      </c>
+      <c r="O21" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="P21" s="5">
+        <v>41115</v>
+      </c>
+      <c r="Q21" s="5">
+        <v>1</v>
+      </c>
+      <c r="R21" s="5">
+        <v>99</v>
+      </c>
+      <c r="S21" s="5">
+        <v>2121463</v>
+      </c>
+      <c r="T21" s="5">
+        <v>88901234567</v>
+      </c>
+      <c r="U21" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="V21" s="5">
+        <v>1</v>
+      </c>
+      <c r="W21" s="5"/>
+      <c r="X21" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="Y21" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="Z21" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA21" s="5">
+        <v>2</v>
+      </c>
+      <c r="AB21" s="5">
+        <v>2</v>
+      </c>
+      <c r="AC21" s="5">
+        <v>13</v>
+      </c>
+      <c r="AD21" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="AE21" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="AF21" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG21" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH21" s="5">
+        <v>2</v>
+      </c>
+      <c r="AI21" s="5">
+        <v>11</v>
+      </c>
+      <c r="AJ21" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="AK21" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL21" s="5">
+        <v>3</v>
+      </c>
+      <c r="AM21" s="5">
+        <v>17</v>
+      </c>
+      <c r="AN21" s="5">
+        <v>12</v>
+      </c>
+      <c r="AO21" s="24" t="s">
+        <v>175</v>
+      </c>
+      <c r="AP21" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ21" s="5">
+        <v>21</v>
+      </c>
+      <c r="AR21" s="5">
+        <v>2008</v>
+      </c>
+      <c r="AS21" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="AT21" s="24" t="s">
+        <v>174</v>
+      </c>
+      <c r="AU21" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="AV21" s="5">
+        <v>2</v>
+      </c>
+      <c r="AW21" s="5">
+        <v>7000000</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4536,6 +6268,17 @@
     <hyperlink ref="U8" r:id="rId9" display="dina@gmail.com"/>
     <hyperlink ref="U9" r:id="rId10" display="hendra@gmail.com"/>
     <hyperlink ref="U10" r:id="rId11" display="sandraputri@gmail.com"/>
+    <hyperlink ref="U11" r:id="rId12" display="dimasd132y99@gmail.com" tooltip="mailto:dimasd132y99@gmail.com"/>
+    <hyperlink ref="U12" r:id="rId13" display="sa132iayudha262@gmail.com" tooltip="mailto:sa132iayudha262@gmail.com"/>
+    <hyperlink ref="U13" r:id="rId14" display="ba123ar@gmail.com" tooltip="mailto:ba123ar@gmail.com"/>
+    <hyperlink ref="U14" r:id="rId15" display="an123tian20@gmail.com" tooltip="mailto:an123tian20@gmail.com"/>
+    <hyperlink ref="U15" r:id="rId16" display="rinap132@gmail.com" tooltip="mailto:rinap132@gmail.com"/>
+    <hyperlink ref="U16" r:id="rId17" display="andiw312@gmail.com" tooltip="mailto:andiw312@gmail.com"/>
+    <hyperlink ref="U17" r:id="rId18" display="dina132@gmail.com" tooltip="mailto:dina132@gmail.com"/>
+    <hyperlink ref="U18" r:id="rId19" display="hendr132a@gmail.com" tooltip="mailto:hendr132a@gmail.com"/>
+    <hyperlink ref="U19" r:id="rId20" display="sandra123putri@gmail.com" tooltip="mailto:sandra123putri@gmail.com"/>
+    <hyperlink ref="U20" r:id="rId21" display="sandra132putri@gmail.com" tooltip="mailto:sandra132putri@gmail.com"/>
+    <hyperlink ref="U21" r:id="rId22" display="sandrapu132tri@gmail.com" tooltip="mailto:sandrapu132tri@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
refactor : UUID to AI id
</commit_message>
<xml_diff>
--- a/public/template/template_import_mahasiswa.xlsx
+++ b/public/template/template_import_mahasiswa.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
@@ -1132,7 +1132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2289" uniqueCount="1460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2386" uniqueCount="1460">
   <si>
     <t>NIM</t>
   </si>
@@ -1314,7 +1314,7 @@
     <t>2018-03-20</t>
   </si>
   <si>
-    <t>20221</t>
+    <t>20241</t>
   </si>
   <si>
     <t>Jl. Bahagia, RT 2 RW 3, Bunga, Cempaka Adimulyo</t>
@@ -6737,6 +6737,13 @@
 </styleSheet>
 </file>
 
+<file path=xl/customStorage/customStorage.xml><?xml version="1.0" encoding="utf-8"?>
+<customStorage xmlns="https://web.wps.cn/et/2018/main">
+  <book/>
+  <sheets/>
+</customStorage>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -6997,8 +7004,8 @@
   <sheetPr/>
   <dimension ref="A1:AW101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6:N101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1047619047619" defaultRowHeight="15"/>
@@ -7371,7 +7378,7 @@
         <v>43728</v>
       </c>
       <c r="N3" s="4">
-        <v>20221</v>
+        <v>20241</v>
       </c>
       <c r="O3" s="4" t="s">
         <v>61</v>
@@ -7517,8 +7524,8 @@
       <c r="M4" s="17">
         <v>43840</v>
       </c>
-      <c r="N4" s="4">
-        <v>20221</v>
+      <c r="N4" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O4" s="4" t="s">
         <v>61</v>
@@ -7664,8 +7671,8 @@
       <c r="M5" s="17">
         <v>43707</v>
       </c>
-      <c r="N5" s="4">
-        <v>20221</v>
+      <c r="N5" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O5" s="4" t="s">
         <v>61</v>
@@ -7811,8 +7818,8 @@
       <c r="M6" s="17">
         <v>43348</v>
       </c>
-      <c r="N6" s="4">
-        <v>20221</v>
+      <c r="N6" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O6" s="4" t="s">
         <v>61</v>
@@ -7958,8 +7965,8 @@
       <c r="M7" s="17">
         <v>43850</v>
       </c>
-      <c r="N7" s="4">
-        <v>20221</v>
+      <c r="N7" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O7" s="4" t="s">
         <v>61</v>
@@ -8105,8 +8112,8 @@
       <c r="M8" s="17">
         <v>43539</v>
       </c>
-      <c r="N8" s="4">
-        <v>20221</v>
+      <c r="N8" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O8" s="4" t="s">
         <v>61</v>
@@ -8252,8 +8259,8 @@
       <c r="M9" s="17">
         <v>43889</v>
       </c>
-      <c r="N9" s="4">
-        <v>20221</v>
+      <c r="N9" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O9" s="4" t="s">
         <v>61</v>
@@ -8399,8 +8406,8 @@
       <c r="M10" s="17">
         <v>43606</v>
       </c>
-      <c r="N10" s="4">
-        <v>20221</v>
+      <c r="N10" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O10" s="4" t="s">
         <v>61</v>
@@ -8693,8 +8700,8 @@
       <c r="M12" s="17">
         <v>43728</v>
       </c>
-      <c r="N12" s="4">
-        <v>20221</v>
+      <c r="N12" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O12" s="4" t="s">
         <v>61</v>
@@ -8840,8 +8847,8 @@
       <c r="M13" s="17">
         <v>43840</v>
       </c>
-      <c r="N13" s="4">
-        <v>20221</v>
+      <c r="N13" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O13" s="4" t="s">
         <v>61</v>
@@ -8987,8 +8994,8 @@
       <c r="M14" s="17">
         <v>43707</v>
       </c>
-      <c r="N14" s="4">
-        <v>20221</v>
+      <c r="N14" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O14" s="4" t="s">
         <v>61</v>
@@ -9134,8 +9141,8 @@
       <c r="M15" s="17">
         <v>43348</v>
       </c>
-      <c r="N15" s="4">
-        <v>20221</v>
+      <c r="N15" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O15" s="4" t="s">
         <v>61</v>
@@ -9281,8 +9288,8 @@
       <c r="M16" s="17">
         <v>43850</v>
       </c>
-      <c r="N16" s="4">
-        <v>20221</v>
+      <c r="N16" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O16" s="4" t="s">
         <v>61</v>
@@ -9428,8 +9435,8 @@
       <c r="M17" s="17">
         <v>43539</v>
       </c>
-      <c r="N17" s="4">
-        <v>20221</v>
+      <c r="N17" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O17" s="4" t="s">
         <v>61</v>
@@ -9575,8 +9582,8 @@
       <c r="M18" s="17">
         <v>43889</v>
       </c>
-      <c r="N18" s="4">
-        <v>20221</v>
+      <c r="N18" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O18" s="4" t="s">
         <v>61</v>
@@ -9722,8 +9729,8 @@
       <c r="M19" s="17">
         <v>43606</v>
       </c>
-      <c r="N19" s="4">
-        <v>20221</v>
+      <c r="N19" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O19" s="4" t="s">
         <v>61</v>
@@ -9869,8 +9876,8 @@
       <c r="M20" s="17">
         <v>43606</v>
       </c>
-      <c r="N20" s="4">
-        <v>20221</v>
+      <c r="N20" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O20" s="4" t="s">
         <v>61</v>
@@ -10016,8 +10023,8 @@
       <c r="M21" s="19">
         <v>43606</v>
       </c>
-      <c r="N21" s="6">
-        <v>20221</v>
+      <c r="N21" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O21" s="6" t="s">
         <v>61</v>
@@ -10163,8 +10170,8 @@
       <c r="M22" t="s">
         <v>215</v>
       </c>
-      <c r="N22">
-        <v>20221</v>
+      <c r="N22" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O22" t="s">
         <v>216</v>
@@ -10309,8 +10316,8 @@
       <c r="M23" t="s">
         <v>232</v>
       </c>
-      <c r="N23">
-        <v>20221</v>
+      <c r="N23" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O23" t="s">
         <v>233</v>
@@ -10455,8 +10462,8 @@
       <c r="M24" t="s">
         <v>250</v>
       </c>
-      <c r="N24">
-        <v>20221</v>
+      <c r="N24" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O24" t="s">
         <v>251</v>
@@ -10601,8 +10608,8 @@
       <c r="M25" t="s">
         <v>266</v>
       </c>
-      <c r="N25">
-        <v>20221</v>
+      <c r="N25" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O25" t="s">
         <v>267</v>
@@ -10747,8 +10754,8 @@
       <c r="M26" t="s">
         <v>283</v>
       </c>
-      <c r="N26">
-        <v>20221</v>
+      <c r="N26" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O26" t="s">
         <v>284</v>
@@ -10893,8 +10900,8 @@
       <c r="M27" t="s">
         <v>300</v>
       </c>
-      <c r="N27">
-        <v>20221</v>
+      <c r="N27" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O27" t="s">
         <v>301</v>
@@ -11039,8 +11046,8 @@
       <c r="M28" t="s">
         <v>317</v>
       </c>
-      <c r="N28">
-        <v>20221</v>
+      <c r="N28" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O28" t="s">
         <v>318</v>
@@ -11185,8 +11192,8 @@
       <c r="M29" t="s">
         <v>333</v>
       </c>
-      <c r="N29">
-        <v>20221</v>
+      <c r="N29" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O29" t="s">
         <v>334</v>
@@ -11331,8 +11338,8 @@
       <c r="M30" t="s">
         <v>349</v>
       </c>
-      <c r="N30">
-        <v>20221</v>
+      <c r="N30" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O30" t="s">
         <v>350</v>
@@ -11477,8 +11484,8 @@
       <c r="M31" t="s">
         <v>365</v>
       </c>
-      <c r="N31">
-        <v>20221</v>
+      <c r="N31" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O31" t="s">
         <v>366</v>
@@ -11623,8 +11630,8 @@
       <c r="M32" t="s">
         <v>381</v>
       </c>
-      <c r="N32">
-        <v>20221</v>
+      <c r="N32" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O32" t="s">
         <v>382</v>
@@ -11769,8 +11776,8 @@
       <c r="M33" t="s">
         <v>398</v>
       </c>
-      <c r="N33">
-        <v>20221</v>
+      <c r="N33" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O33" t="s">
         <v>399</v>
@@ -11915,8 +11922,8 @@
       <c r="M34" t="s">
         <v>414</v>
       </c>
-      <c r="N34">
-        <v>20221</v>
+      <c r="N34" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O34" t="s">
         <v>415</v>
@@ -12061,8 +12068,8 @@
       <c r="M35" t="s">
         <v>430</v>
       </c>
-      <c r="N35">
-        <v>20221</v>
+      <c r="N35" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O35" t="s">
         <v>431</v>
@@ -12207,8 +12214,8 @@
       <c r="M36" t="s">
         <v>446</v>
       </c>
-      <c r="N36">
-        <v>20221</v>
+      <c r="N36" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O36" t="s">
         <v>447</v>
@@ -12353,8 +12360,8 @@
       <c r="M37" t="s">
         <v>462</v>
       </c>
-      <c r="N37">
-        <v>20221</v>
+      <c r="N37" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O37" t="s">
         <v>463</v>
@@ -12499,8 +12506,8 @@
       <c r="M38" t="s">
         <v>478</v>
       </c>
-      <c r="N38">
-        <v>20221</v>
+      <c r="N38" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O38" t="s">
         <v>479</v>
@@ -12645,8 +12652,8 @@
       <c r="M39" t="s">
         <v>494</v>
       </c>
-      <c r="N39">
-        <v>20221</v>
+      <c r="N39" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O39" t="s">
         <v>495</v>
@@ -12791,8 +12798,8 @@
       <c r="M40" t="s">
         <v>510</v>
       </c>
-      <c r="N40">
-        <v>20221</v>
+      <c r="N40" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O40" t="s">
         <v>511</v>
@@ -12937,8 +12944,8 @@
       <c r="M41" t="s">
         <v>526</v>
       </c>
-      <c r="N41">
-        <v>20221</v>
+      <c r="N41" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O41" t="s">
         <v>527</v>
@@ -13083,8 +13090,8 @@
       <c r="M42" t="s">
         <v>541</v>
       </c>
-      <c r="N42">
-        <v>20221</v>
+      <c r="N42" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O42" t="s">
         <v>542</v>
@@ -13229,8 +13236,8 @@
       <c r="M43" t="s">
         <v>557</v>
       </c>
-      <c r="N43">
-        <v>20221</v>
+      <c r="N43" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O43" t="s">
         <v>558</v>
@@ -13375,8 +13382,8 @@
       <c r="M44" t="s">
         <v>573</v>
       </c>
-      <c r="N44">
-        <v>20221</v>
+      <c r="N44" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O44" t="s">
         <v>574</v>
@@ -13521,8 +13528,8 @@
       <c r="M45" t="s">
         <v>589</v>
       </c>
-      <c r="N45">
-        <v>20221</v>
+      <c r="N45" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O45" t="s">
         <v>590</v>
@@ -13667,8 +13674,8 @@
       <c r="M46" t="s">
         <v>604</v>
       </c>
-      <c r="N46">
-        <v>20221</v>
+      <c r="N46" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O46" t="s">
         <v>605</v>
@@ -13813,8 +13820,8 @@
       <c r="M47" t="s">
         <v>619</v>
       </c>
-      <c r="N47">
-        <v>20221</v>
+      <c r="N47" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O47" t="s">
         <v>620</v>
@@ -13959,8 +13966,8 @@
       <c r="M48" t="s">
         <v>634</v>
       </c>
-      <c r="N48">
-        <v>20221</v>
+      <c r="N48" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O48" t="s">
         <v>635</v>
@@ -14105,8 +14112,8 @@
       <c r="M49" t="s">
         <v>649</v>
       </c>
-      <c r="N49">
-        <v>20221</v>
+      <c r="N49" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O49" t="s">
         <v>650</v>
@@ -14251,8 +14258,8 @@
       <c r="M50" t="s">
         <v>665</v>
       </c>
-      <c r="N50">
-        <v>20221</v>
+      <c r="N50" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O50" t="s">
         <v>666</v>
@@ -14397,8 +14404,8 @@
       <c r="M51" t="s">
         <v>680</v>
       </c>
-      <c r="N51">
-        <v>20221</v>
+      <c r="N51" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O51" t="s">
         <v>681</v>
@@ -14543,8 +14550,8 @@
       <c r="M52" t="s">
         <v>695</v>
       </c>
-      <c r="N52">
-        <v>20221</v>
+      <c r="N52" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O52" t="s">
         <v>696</v>
@@ -14689,8 +14696,8 @@
       <c r="M53" t="s">
         <v>365</v>
       </c>
-      <c r="N53">
-        <v>20221</v>
+      <c r="N53" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O53" t="s">
         <v>710</v>
@@ -14835,8 +14842,8 @@
       <c r="M54" t="s">
         <v>724</v>
       </c>
-      <c r="N54">
-        <v>20221</v>
+      <c r="N54" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O54" t="s">
         <v>725</v>
@@ -14981,8 +14988,8 @@
       <c r="M55" t="s">
         <v>740</v>
       </c>
-      <c r="N55">
-        <v>20221</v>
+      <c r="N55" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O55" t="s">
         <v>741</v>
@@ -15127,8 +15134,8 @@
       <c r="M56" t="s">
         <v>755</v>
       </c>
-      <c r="N56">
-        <v>20221</v>
+      <c r="N56" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O56" t="s">
         <v>756</v>
@@ -15273,8 +15280,8 @@
       <c r="M57" t="s">
         <v>771</v>
       </c>
-      <c r="N57">
-        <v>20221</v>
+      <c r="N57" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O57" t="s">
         <v>772</v>
@@ -15419,8 +15426,8 @@
       <c r="M58" t="s">
         <v>787</v>
       </c>
-      <c r="N58">
-        <v>20221</v>
+      <c r="N58" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O58" t="s">
         <v>788</v>
@@ -15565,8 +15572,8 @@
       <c r="M59" t="s">
         <v>802</v>
       </c>
-      <c r="N59">
-        <v>20221</v>
+      <c r="N59" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O59" t="s">
         <v>803</v>
@@ -15711,8 +15718,8 @@
       <c r="M60" t="s">
         <v>818</v>
       </c>
-      <c r="N60">
-        <v>20221</v>
+      <c r="N60" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O60" t="s">
         <v>819</v>
@@ -15857,8 +15864,8 @@
       <c r="M61" t="s">
         <v>834</v>
       </c>
-      <c r="N61">
-        <v>20221</v>
+      <c r="N61" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O61" t="s">
         <v>835</v>
@@ -16003,8 +16010,8 @@
       <c r="M62" t="s">
         <v>849</v>
       </c>
-      <c r="N62">
-        <v>20221</v>
+      <c r="N62" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O62" t="s">
         <v>850</v>
@@ -16149,8 +16156,8 @@
       <c r="M63" t="s">
         <v>865</v>
       </c>
-      <c r="N63">
-        <v>20221</v>
+      <c r="N63" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O63" t="s">
         <v>866</v>
@@ -16295,8 +16302,8 @@
       <c r="M64" t="s">
         <v>879</v>
       </c>
-      <c r="N64">
-        <v>20221</v>
+      <c r="N64" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O64" t="s">
         <v>880</v>
@@ -16441,8 +16448,8 @@
       <c r="M65" t="s">
         <v>895</v>
       </c>
-      <c r="N65">
-        <v>20221</v>
+      <c r="N65" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O65" t="s">
         <v>896</v>
@@ -16587,8 +16594,8 @@
       <c r="M66" t="s">
         <v>910</v>
       </c>
-      <c r="N66">
-        <v>20221</v>
+      <c r="N66" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O66" t="s">
         <v>911</v>
@@ -16733,8 +16740,8 @@
       <c r="M67" t="s">
         <v>926</v>
       </c>
-      <c r="N67">
-        <v>20221</v>
+      <c r="N67" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O67" t="s">
         <v>927</v>
@@ -16879,8 +16886,8 @@
       <c r="M68" t="s">
         <v>942</v>
       </c>
-      <c r="N68">
-        <v>20221</v>
+      <c r="N68" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O68" t="s">
         <v>943</v>
@@ -17025,8 +17032,8 @@
       <c r="M69" t="s">
         <v>958</v>
       </c>
-      <c r="N69">
-        <v>20221</v>
+      <c r="N69" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O69" t="s">
         <v>959</v>
@@ -17171,8 +17178,8 @@
       <c r="M70" t="s">
         <v>974</v>
       </c>
-      <c r="N70">
-        <v>20221</v>
+      <c r="N70" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O70" t="s">
         <v>975</v>
@@ -17317,8 +17324,8 @@
       <c r="M71" t="s">
         <v>990</v>
       </c>
-      <c r="N71">
-        <v>20221</v>
+      <c r="N71" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O71" t="s">
         <v>991</v>
@@ -17463,8 +17470,8 @@
       <c r="M72" t="s">
         <v>1005</v>
       </c>
-      <c r="N72">
-        <v>20221</v>
+      <c r="N72" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O72" t="s">
         <v>1006</v>
@@ -17609,8 +17616,8 @@
       <c r="M73" t="s">
         <v>1021</v>
       </c>
-      <c r="N73">
-        <v>20221</v>
+      <c r="N73" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O73" t="s">
         <v>1022</v>
@@ -17755,8 +17762,8 @@
       <c r="M74" t="s">
         <v>1037</v>
       </c>
-      <c r="N74">
-        <v>20221</v>
+      <c r="N74" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O74" t="s">
         <v>1038</v>
@@ -17901,8 +17908,8 @@
       <c r="M75" t="s">
         <v>1053</v>
       </c>
-      <c r="N75">
-        <v>20221</v>
+      <c r="N75" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O75" t="s">
         <v>1054</v>
@@ -18047,8 +18054,8 @@
       <c r="M76" t="s">
         <v>1069</v>
       </c>
-      <c r="N76">
-        <v>20221</v>
+      <c r="N76" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O76" t="s">
         <v>1070</v>
@@ -18193,8 +18200,8 @@
       <c r="M77" t="s">
         <v>1085</v>
       </c>
-      <c r="N77">
-        <v>20221</v>
+      <c r="N77" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O77" t="s">
         <v>1086</v>
@@ -18339,8 +18346,8 @@
       <c r="M78" t="s">
         <v>1101</v>
       </c>
-      <c r="N78">
-        <v>20221</v>
+      <c r="N78" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O78" t="s">
         <v>1102</v>
@@ -18485,8 +18492,8 @@
       <c r="M79" t="s">
         <v>1116</v>
       </c>
-      <c r="N79">
-        <v>20221</v>
+      <c r="N79" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O79" t="s">
         <v>1117</v>
@@ -18631,8 +18638,8 @@
       <c r="M80" t="s">
         <v>1132</v>
       </c>
-      <c r="N80">
-        <v>20221</v>
+      <c r="N80" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O80" t="s">
         <v>1133</v>
@@ -18777,8 +18784,8 @@
       <c r="M81" t="s">
         <v>1148</v>
       </c>
-      <c r="N81">
-        <v>20221</v>
+      <c r="N81" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O81" t="s">
         <v>1149</v>
@@ -18923,8 +18930,8 @@
       <c r="M82" t="s">
         <v>1163</v>
       </c>
-      <c r="N82">
-        <v>20221</v>
+      <c r="N82" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O82" t="s">
         <v>1164</v>
@@ -19069,8 +19076,8 @@
       <c r="M83" t="s">
         <v>1178</v>
       </c>
-      <c r="N83">
-        <v>20221</v>
+      <c r="N83" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O83" t="s">
         <v>1179</v>
@@ -19215,8 +19222,8 @@
       <c r="M84" t="s">
         <v>1193</v>
       </c>
-      <c r="N84">
-        <v>20221</v>
+      <c r="N84" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O84" t="s">
         <v>1194</v>
@@ -19361,8 +19368,8 @@
       <c r="M85" t="s">
         <v>1209</v>
       </c>
-      <c r="N85">
-        <v>20221</v>
+      <c r="N85" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O85" t="s">
         <v>1210</v>
@@ -19507,8 +19514,8 @@
       <c r="M86" t="s">
         <v>771</v>
       </c>
-      <c r="N86">
-        <v>20221</v>
+      <c r="N86" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O86" t="s">
         <v>1224</v>
@@ -19653,8 +19660,8 @@
       <c r="M87" t="s">
         <v>1237</v>
       </c>
-      <c r="N87">
-        <v>20221</v>
+      <c r="N87" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O87" t="s">
         <v>1238</v>
@@ -19799,8 +19806,8 @@
       <c r="M88" t="s">
         <v>1253</v>
       </c>
-      <c r="N88">
-        <v>20221</v>
+      <c r="N88" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O88" t="s">
         <v>1254</v>
@@ -19945,8 +19952,8 @@
       <c r="M89" t="s">
         <v>1269</v>
       </c>
-      <c r="N89">
-        <v>20221</v>
+      <c r="N89" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O89" t="s">
         <v>1270</v>
@@ -20091,8 +20098,8 @@
       <c r="M90" t="s">
         <v>1285</v>
       </c>
-      <c r="N90">
-        <v>20221</v>
+      <c r="N90" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O90" t="s">
         <v>1286</v>
@@ -20237,8 +20244,8 @@
       <c r="M91" t="s">
         <v>1300</v>
       </c>
-      <c r="N91">
-        <v>20221</v>
+      <c r="N91" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O91" t="s">
         <v>1301</v>
@@ -20383,8 +20390,8 @@
       <c r="M92" t="s">
         <v>1316</v>
       </c>
-      <c r="N92">
-        <v>20221</v>
+      <c r="N92" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O92" t="s">
         <v>1317</v>
@@ -20529,8 +20536,8 @@
       <c r="M93" t="s">
         <v>1329</v>
       </c>
-      <c r="N93">
-        <v>20221</v>
+      <c r="N93" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O93" t="s">
         <v>1330</v>
@@ -20675,8 +20682,8 @@
       <c r="M94" t="s">
         <v>1344</v>
       </c>
-      <c r="N94">
-        <v>20221</v>
+      <c r="N94" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O94" t="s">
         <v>1345</v>
@@ -20821,8 +20828,8 @@
       <c r="M95" t="s">
         <v>1360</v>
       </c>
-      <c r="N95">
-        <v>20221</v>
+      <c r="N95" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O95" t="s">
         <v>1361</v>
@@ -20967,8 +20974,8 @@
       <c r="M96" t="s">
         <v>1375</v>
       </c>
-      <c r="N96">
-        <v>20221</v>
+      <c r="N96" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O96" t="s">
         <v>1376</v>
@@ -21113,8 +21120,8 @@
       <c r="M97" t="s">
         <v>1391</v>
       </c>
-      <c r="N97">
-        <v>20221</v>
+      <c r="N97" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O97" t="s">
         <v>1392</v>
@@ -21259,8 +21266,8 @@
       <c r="M98" t="s">
         <v>1406</v>
       </c>
-      <c r="N98">
-        <v>20221</v>
+      <c r="N98" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O98" t="s">
         <v>1407</v>
@@ -21405,8 +21412,8 @@
       <c r="M99" t="s">
         <v>1178</v>
       </c>
-      <c r="N99">
-        <v>20221</v>
+      <c r="N99" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O99" t="s">
         <v>1421</v>
@@ -21551,8 +21558,8 @@
       <c r="M100" t="s">
         <v>1435</v>
       </c>
-      <c r="N100">
-        <v>20221</v>
+      <c r="N100" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O100" t="s">
         <v>1436</v>
@@ -21697,8 +21704,8 @@
       <c r="M101" t="s">
         <v>1450</v>
       </c>
-      <c r="N101">
-        <v>20221</v>
+      <c r="N101" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="O101" t="s">
         <v>1451</v>

</xml_diff>